<commit_message>
update scatter to include all data
</commit_message>
<xml_diff>
--- a/data/mountain.xlsx
+++ b/data/mountain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walker/Library/CloudStorage/GoogleDrive-walker@maine.edu/My Drive/Github projects/Bike Geometry Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524FCF50-2FBC-BC49-BE35-85A69F489A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CEC44-AFF2-2748-A534-FEB642FF83DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="780" windowWidth="27640" windowHeight="16440" activeTab="3" xr2:uid="{7F4EF72F-20E3-5949-863E-8288BFE4110E}"/>
+    <workbookView xWindow="6260" yWindow="780" windowWidth="27640" windowHeight="16440" activeTab="2" xr2:uid="{7F4EF72F-20E3-5949-863E-8288BFE4110E}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Trek Procaliber 2019" sheetId="4" r:id="rId4"/>
     <sheet name="Trek Procaliber 2023" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -759,6 +762,234 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="bikeinsights"/>
+      <sheetName val="Alchemy Rogue 2022"/>
+      <sheetName val="All-City Cosmic Stallion 2022"/>
+      <sheetName val="All-City Gorilla Monsoon 2022"/>
+      <sheetName val="Alle Bike MB31 Bramley 2022"/>
+      <sheetName val="Amigo Bug Out 2022"/>
+      <sheetName val="Argonaut GR3 2023"/>
+      <sheetName val="Bearclaw Beaux Jaxon 2022"/>
+      <sheetName val="Blackheart All Road TI 2022"/>
+      <sheetName val="BlackMtnCy La Cabra 2022"/>
+      <sheetName val="BlackMtnCy Monstercross V5 2022"/>
+      <sheetName val="Bombtrack Beyond 2 2022"/>
+      <sheetName val="Bombtrack Beyond+ Adv 2022"/>
+      <sheetName val="Bombtrack Hook 2022"/>
+      <sheetName val="BMC URS AL 2022"/>
+      <sheetName val="BMC URS AL SUS 2022"/>
+      <sheetName val="BMC URS One 2022"/>
+      <sheetName val="Breezer Radar X Pro 2022"/>
+      <sheetName val="Calfee"/>
+      <sheetName val="Cannondale SuperSix Evo 2022"/>
+      <sheetName val="Canyon Grail 7 1by 2022"/>
+      <sheetName val="Canyon Grail SL 2022"/>
+      <sheetName val="Canyon Grizl 7 1by 2022"/>
+      <sheetName val="Cervelo Aspero 2022"/>
+      <sheetName val="Chiru Kegeti 2022"/>
+      <sheetName val="Chumba Terlingua steel fdo 2022"/>
+      <sheetName val="Chumba Yaupon 2022"/>
+      <sheetName val="Cinelli Hobootleg Geo 2022"/>
+      <sheetName val="Cotic Cascade 2022"/>
+      <sheetName val="Devinci Hatchet 2022"/>
+      <sheetName val="Enigma Escape Flat-bar 2022"/>
+      <sheetName val="Evil Chamois Hagar GRX 2022"/>
+      <sheetName val="Fezzari Shafer 2022"/>
+      <sheetName val="Fiftyone Assassin short-hi 2022"/>
+      <sheetName val="Fiftyone Assassin long-low 2022"/>
+      <sheetName val="Focus Atlas 8.9 2023"/>
+      <sheetName val="Fustle Causway GR1 2022"/>
+      <sheetName val="Genesis Vagabond 2022"/>
+      <sheetName val="Giant Revolt X pro 1 long 2023"/>
+      <sheetName val="Giant Revolt X pro 1 short 2023"/>
+      <sheetName val="Hudski Doggler Gravel 2022"/>
+      <sheetName val="Ibis Hakka MX 2023"/>
+      <sheetName val="Kanzo Adventure New 2022"/>
+      <sheetName val="Knolly Cache Steel 2022"/>
+      <sheetName val="Kona Sutra ULTD 2022"/>
+      <sheetName val="Lauf Siegla 2022"/>
+      <sheetName val="Light Blue Darwin 2022"/>
+      <sheetName val="Liz Devote Advance 2023"/>
+      <sheetName val="Marin DSX 2 2022"/>
+      <sheetName val="Mason InSearchOf 2022"/>
+      <sheetName val="Merida Silex 2022"/>
+      <sheetName val="Moots Routt ESC 2022"/>
+      <sheetName val="Mosaic GT-1X 2022"/>
+      <sheetName val="Niner RLT 9 RDO 2022"/>
+      <sheetName val="No22 Drifter X 2022"/>
+      <sheetName val="Noble GX 5 2022"/>
+      <sheetName val="Nordest Kutxo 2022"/>
+      <sheetName val="Obed Boundary 2022"/>
+      <sheetName val="OPEN U.P. 2022"/>
+      <sheetName val="Open WI.DE 2022"/>
+      <sheetName val="Orbea Terra M 2023"/>
+      <sheetName val="Orbea Terra H 2023"/>
+      <sheetName val="Otso Fenrir 2022"/>
+      <sheetName val="Otso Waheela C front 2022"/>
+      <sheetName val="Otso Waheela C rear 2022"/>
+      <sheetName val="Otso Warakin Stainless 2022"/>
+      <sheetName val="Panorama Taiga EXP 2022"/>
+      <sheetName val="Pinarello Grevil F 2023"/>
+      <sheetName val="Reeb Sams Pants 2022"/>
+      <sheetName val="Revel Rover 2022"/>
+      <sheetName val="Ribble Gravel SL 2022"/>
+      <sheetName val="Ritchey Outback frameset 2022"/>
+      <sheetName val="Rondo MYLC CF Hi 2022"/>
+      <sheetName val="Rose Backroad XPLR 2022"/>
+      <sheetName val="Rondo MYLC CF Lo 2022"/>
+      <sheetName val="Salsa Cutthroat 2022"/>
+      <sheetName val="Salsa Fargo rear dropout 2022"/>
+      <sheetName val="Salsa Fargo front dropout 2022"/>
+      <sheetName val="Salsa Vaya 2022"/>
+      <sheetName val="Salsa Warbird 2022"/>
+      <sheetName val="Santa Cruz Stigmata 2022"/>
+      <sheetName val="Scott Addict Gravel 10 2022"/>
+      <sheetName val="Shand Stooshie 2022"/>
+      <sheetName val="Solace OM-3 Short 2022"/>
+      <sheetName val="Soma Wolverine 2022"/>
+      <sheetName val="Sonder Camino AL 2022"/>
+      <sheetName val="Specialized Diverge 2022"/>
+      <sheetName val="Specialized Diverge Evo 2022"/>
+      <sheetName val="Specialized Diverge STR 2023"/>
+      <sheetName val="Squid Gravtron 2022"/>
+      <sheetName val="Surly Ghost Grappler 2022"/>
+      <sheetName val="Thesis OB1 2022"/>
+      <sheetName val="Tout Terrain Scrambler 28 2022"/>
+      <sheetName val="Trek Boone 6 2022"/>
+      <sheetName val="Trek Checkpoint SL5 2022"/>
+      <sheetName val="Tumbleweed Stargazer 2022"/>
+      <sheetName val="Ventum GS1 2023"/>
+      <sheetName val="Why R+ V4 2022"/>
+      <sheetName val="Whyte Friston Gravel 2022"/>
+      <sheetName val="Whyte Gisburn 2022"/>
+      <sheetName val="Wilde Rambler SL 2023"/>
+      <sheetName val="Wilier Jena 2022"/>
+      <sheetName val="Wilier Rave SLR 2022"/>
+      <sheetName val="YT Szepter 2023"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+      <sheetData sheetId="62" refreshError="1"/>
+      <sheetData sheetId="63" refreshError="1"/>
+      <sheetData sheetId="64" refreshError="1"/>
+      <sheetData sheetId="65" refreshError="1"/>
+      <sheetData sheetId="66" refreshError="1"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
+      <sheetData sheetId="69" refreshError="1"/>
+      <sheetData sheetId="70" refreshError="1"/>
+      <sheetData sheetId="71" refreshError="1"/>
+      <sheetData sheetId="72" refreshError="1"/>
+      <sheetData sheetId="73" refreshError="1"/>
+      <sheetData sheetId="74" refreshError="1"/>
+      <sheetData sheetId="75" refreshError="1"/>
+      <sheetData sheetId="76" refreshError="1"/>
+      <sheetData sheetId="77" refreshError="1"/>
+      <sheetData sheetId="78" refreshError="1"/>
+      <sheetData sheetId="79" refreshError="1"/>
+      <sheetData sheetId="80" refreshError="1"/>
+      <sheetData sheetId="81" refreshError="1"/>
+      <sheetData sheetId="82" refreshError="1"/>
+      <sheetData sheetId="83" refreshError="1"/>
+      <sheetData sheetId="84" refreshError="1"/>
+      <sheetData sheetId="85" refreshError="1"/>
+      <sheetData sheetId="86" refreshError="1"/>
+      <sheetData sheetId="87" refreshError="1"/>
+      <sheetData sheetId="88" refreshError="1"/>
+      <sheetData sheetId="89" refreshError="1"/>
+      <sheetData sheetId="90" refreshError="1"/>
+      <sheetData sheetId="91" refreshError="1"/>
+      <sheetData sheetId="92" refreshError="1"/>
+      <sheetData sheetId="93" refreshError="1"/>
+      <sheetData sheetId="94" refreshError="1"/>
+      <sheetData sheetId="95" refreshError="1"/>
+      <sheetData sheetId="96">
+        <row r="2">
+          <cell r="D2">
+            <v>506</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="97" refreshError="1"/>
+      <sheetData sheetId="98" refreshError="1"/>
+      <sheetData sheetId="99" refreshError="1"/>
+      <sheetData sheetId="100" refreshError="1"/>
+      <sheetData sheetId="101" refreshError="1"/>
+      <sheetData sheetId="102" refreshError="1"/>
+      <sheetData sheetId="103" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,7 +1420,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2399,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645B082A-C36B-8F42-900D-0EA4FD30DA59}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2440,12 +2671,12 @@
         <f>B30</f>
         <v>Crank Length</v>
       </c>
-      <c r="C2" s="7">
-        <f t="shared" ref="C2:G2" si="0">IF(RIGHT(C30,1)="m",VALUE(MID(C30,1,LEN(C30)-2)),VALUE(MID(C30,1,LEN(C30)-1)))</f>
-        <v>165</v>
+      <c r="C2" s="7" t="b">
+        <f>'[1]Ventum GS1 2023'!$D$2=IF(RIGHT(C30,1)="m",VALUE(MID(C30,1,LEN(C30)-2)),VALUE(MID(C30,1,LEN(C30)-1)))</f>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C2:G2" si="0">IF(RIGHT(D30,1)="m",VALUE(MID(D30,1,LEN(D30)-2)),VALUE(MID(D30,1,LEN(D30)-1)))</f>
         <v>170</v>
       </c>
       <c r="E2" s="7">
@@ -3649,7 +3880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B69FD6-D54C-D944-B7D6-1F2D0448CAA0}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -5193,7 +5424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6F7009-C2AE-9046-9C57-3B1E87BD1A83}">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>